<commit_message>
Updating Lesson 24 Spreadsheet.
</commit_message>
<xml_diff>
--- a/lecture/code/LUT.xlsx
+++ b/lecture/code/LUT.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="7515" windowHeight="7425" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="7515" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="4pt sqrt" sheetId="5" r:id="rId1"/>
     <sheet name="8pt sqrt" sheetId="1" r:id="rId2"/>
+    <sheet name="LUT Practice" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>X</t>
   </si>
@@ -52,12 +53,72 @@
   <si>
     <t>base + offset*delta</t>
   </si>
+  <si>
+    <t>Lut Index</t>
+  </si>
+  <si>
+    <t>Lut Value</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Bin Index</t>
+  </si>
+  <si>
+    <t>Dec Index</t>
+  </si>
+  <si>
+    <t>Trunc Dec Index</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Binary Delta</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Bin Offset</t>
+  </si>
+  <si>
+    <t>Offset*Delta</t>
+  </si>
+  <si>
+    <t>Base + Offset*Delta</t>
+  </si>
+  <si>
+    <t>Final Value</t>
+  </si>
+  <si>
+    <t>175-127 = 42 = 101010</t>
+  </si>
+  <si>
+    <t>0.0000*101010 = 00000.0000</t>
+  </si>
+  <si>
+    <t>127+0 = 127</t>
+  </si>
+  <si>
+    <t>216-175 = 41 = 101001</t>
+  </si>
+  <si>
+    <t>0.1011*101001 = 11100.0011</t>
+  </si>
+  <si>
+    <t>175+28 = 203</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -67,8 +128,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,8 +232,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -162,11 +253,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -182,6 +325,57 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,11 +786,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="41751040"/>
-        <c:axId val="44717696"/>
+        <c:axId val="69002752"/>
+        <c:axId val="69215360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41751040"/>
+        <c:axId val="69002752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -670,7 +864,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44717696"/>
+        <c:crossAx val="69215360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -680,7 +874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44717696"/>
+        <c:axId val="69215360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -764,7 +958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41751040"/>
+        <c:crossAx val="69002752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1247,11 +1441,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="173671936"/>
-        <c:axId val="56281344"/>
+        <c:axId val="69508096"/>
+        <c:axId val="69650304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173671936"/>
+        <c:axId val="69508096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,7 +1519,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56281344"/>
+        <c:crossAx val="69650304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1335,7 +1529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56281344"/>
+        <c:axId val="69650304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1419,7 +1613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173671936"/>
+        <c:crossAx val="69508096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1679,11 +1873,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121075904"/>
-        <c:axId val="121075328"/>
+        <c:axId val="136545024"/>
+        <c:axId val="136546560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121075904"/>
+        <c:axId val="136545024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,12 +1887,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121075328"/>
+        <c:crossAx val="136546560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121075328"/>
+        <c:axId val="136546560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1709,7 +1903,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121075904"/>
+        <c:crossAx val="136545024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3431,11 +3625,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184244224"/>
-        <c:axId val="174099264"/>
+        <c:axId val="139167616"/>
+        <c:axId val="156065792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184244224"/>
+        <c:axId val="139167616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3509,7 +3703,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174099264"/>
+        <c:crossAx val="156065792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3519,7 +3713,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174099264"/>
+        <c:axId val="156065792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3603,7 +3797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184244224"/>
+        <c:crossAx val="139167616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4607,11 +4801,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="173672960"/>
-        <c:axId val="121070720"/>
+        <c:axId val="156098560"/>
+        <c:axId val="156100864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173672960"/>
+        <c:axId val="156098560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4685,7 +4879,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121070720"/>
+        <c:crossAx val="156100864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4695,7 +4889,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121070720"/>
+        <c:axId val="156100864"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4780,7 +4974,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173672960"/>
+        <c:crossAx val="156098560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5293,7 +5487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
@@ -5364,7 +5558,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C2:C4" si="4">$N$6</f>
+        <f t="shared" ref="C3:C4" si="4">$N$6</f>
         <v>0</v>
       </c>
       <c r="D3" s="1">
@@ -5886,8 +6080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36:T42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5926,7 +6120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -5944,7 +6138,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A67" si="3">A3+1</f>
         <v>2</v>
@@ -5971,7 +6165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -5992,7 +6186,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <f>I5*16</f>
+        <f t="shared" ref="J5:J13" si="4">I5*16</f>
         <v>0</v>
       </c>
       <c r="K5" s="1">
@@ -6000,7 +6194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -6021,15 +6215,15 @@
         <v>1</v>
       </c>
       <c r="J6" s="2">
-        <f>I6*16</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" ref="K6:K12" si="4">SQRT(J6)</f>
+        <f t="shared" ref="K6:K12" si="5">SQRT(J6)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -6050,15 +6244,15 @@
         <v>2</v>
       </c>
       <c r="J7" s="3">
-        <f>I7*16</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.6568542494923806</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -6079,15 +6273,15 @@
         <v>3</v>
       </c>
       <c r="J8" s="14">
-        <f>I8*16</f>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="K8" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.9282032302755088</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -6108,15 +6302,15 @@
         <v>4</v>
       </c>
       <c r="J9" s="5">
-        <f>I9*16</f>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="K9" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -6137,15 +6331,15 @@
         <v>5</v>
       </c>
       <c r="J10" s="6">
-        <f>I10*16</f>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="K10" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.9442719099991592</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -6166,15 +6360,15 @@
         <v>6</v>
       </c>
       <c r="J11" s="7">
-        <f>I11*16</f>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
       <c r="K11" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.7979589711327115</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -6195,15 +6389,15 @@
         <v>7</v>
       </c>
       <c r="J12" s="13">
-        <f>I12*16</f>
+        <f t="shared" si="4"/>
         <v>112</v>
       </c>
       <c r="K12" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10.583005244258363</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -6224,7 +6418,7 @@
         <v>8</v>
       </c>
       <c r="J13">
-        <f>I13*16</f>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="K13">
@@ -6232,7 +6426,7 @@
         <v>11.313708498984761</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -6250,7 +6444,7 @@
         <v>0.46410161513775439</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -6268,7 +6462,7 @@
         <v>0.35555127546398912</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -6286,7 +6480,7 @@
         <v>0.24165738677394133</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -6304,7 +6498,7 @@
         <v>0.12298334620741702</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -6350,7 +6544,7 @@
         <v>4.2426406871192848</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" ref="C20:C35" si="5">$K$6 + ($K$7-$K$6)*(A20-$J$6)/16</f>
+        <f t="shared" ref="C20:C34" si="6">$K$6 + ($K$7-$K$6)*(A20-$J$6)/16</f>
         <v>4.2071067811865479</v>
       </c>
       <c r="D20">
@@ -6368,7 +6562,7 @@
         <v>4.358898943540674</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.310660171779821</v>
       </c>
       <c r="D21">
@@ -6386,7 +6580,7 @@
         <v>4.4721359549995796</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.4142135623730949</v>
       </c>
       <c r="D22">
@@ -6404,7 +6598,7 @@
         <v>4.5825756949558398</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5177669529663689</v>
       </c>
       <c r="D23">
@@ -6440,7 +6634,7 @@
         <v>4.7958315233127191</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.7248737341529168</v>
       </c>
       <c r="D25">
@@ -6458,7 +6652,7 @@
         <v>4.8989794855663558</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.8284271247461898</v>
       </c>
       <c r="D26">
@@ -6476,7 +6670,7 @@
         <v>5</v>
       </c>
       <c r="C27" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.9319805153394638</v>
       </c>
       <c r="D27">
@@ -6494,7 +6688,7 @@
         <v>5.0990195135927845</v>
       </c>
       <c r="C28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.0355339059327378</v>
       </c>
       <c r="D28">
@@ -6512,7 +6706,7 @@
         <v>5.196152422706632</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.1390872965260117</v>
       </c>
       <c r="D29">
@@ -6530,7 +6724,7 @@
         <v>5.2915026221291814</v>
       </c>
       <c r="C30" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.2426406871192857</v>
       </c>
       <c r="D30">
@@ -6548,7 +6742,7 @@
         <v>5.3851648071345037</v>
       </c>
       <c r="C31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.3461940777125587</v>
       </c>
       <c r="D31">
@@ -6566,7 +6760,7 @@
         <v>5.4772255750516612</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.4497474683058336</v>
       </c>
       <c r="D32">
@@ -6584,7 +6778,7 @@
         <v>5.5677643628300215</v>
       </c>
       <c r="C33" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.5533008588991066</v>
       </c>
       <c r="D33">
@@ -6602,7 +6796,7 @@
         <v>5.6568542494923806</v>
       </c>
       <c r="C34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.6568542494923806</v>
       </c>
       <c r="D34">
@@ -6638,7 +6832,7 @@
         <v>5.8309518948453007</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" ref="C36:C50" si="6">$K$7 + ($K$8-$K$7)*(A36-$J$7)/16</f>
+        <f t="shared" ref="C36:C50" si="7">$K$7 + ($K$8-$K$7)*(A36-$J$7)/16</f>
         <v>5.8157728720902719</v>
       </c>
       <c r="D36">
@@ -6656,7 +6850,7 @@
         <v>5.9160797830996161</v>
       </c>
       <c r="C37" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.8952321833892167</v>
       </c>
       <c r="D37">
@@ -6674,7 +6868,7 @@
         <v>6</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.9746914946881624</v>
       </c>
       <c r="D38">
@@ -6692,7 +6886,7 @@
         <v>6.0827625302982193</v>
       </c>
       <c r="C39" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.0541508059871081</v>
       </c>
       <c r="D39">
@@ -6710,7 +6904,7 @@
         <v>6.164414002968976</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.1336101172860538</v>
       </c>
       <c r="D40">
@@ -6728,7 +6922,7 @@
         <v>6.2449979983983983</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.2130694285849994</v>
       </c>
       <c r="D41">
@@ -6746,7 +6940,7 @@
         <v>6.324555320336759</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.2925287398839451</v>
       </c>
       <c r="D42">
@@ -6764,7 +6958,7 @@
         <v>6.4031242374328485</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.3719880511828899</v>
       </c>
       <c r="D43">
@@ -6782,7 +6976,7 @@
         <v>6.4807406984078604</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.4514473624818356</v>
       </c>
       <c r="D44">
@@ -6800,7 +6994,7 @@
         <v>6.5574385243020004</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.5309066737807813</v>
       </c>
       <c r="D45">
@@ -6818,7 +7012,7 @@
         <v>6.6332495807107996</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.6103659850797269</v>
       </c>
       <c r="D46">
@@ -6836,7 +7030,7 @@
         <v>6.7082039324993694</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.6898252963786717</v>
       </c>
       <c r="D47">
@@ -6854,7 +7048,7 @@
         <v>6.7823299831252681</v>
       </c>
       <c r="C48" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.7692846076776174</v>
       </c>
       <c r="D48">
@@ -6872,7 +7066,7 @@
         <v>6.8556546004010439</v>
       </c>
       <c r="C49" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.8487439189765631</v>
       </c>
       <c r="D49">
@@ -6890,7 +7084,7 @@
         <v>6.9282032302755088</v>
       </c>
       <c r="C50" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.9282032302755088</v>
       </c>
       <c r="D50">
@@ -6926,7 +7120,7 @@
         <v>7.0710678118654755</v>
       </c>
       <c r="C52" s="14">
-        <f t="shared" ref="C52:C66" si="7">$K$8 + ($K$9-$K$8)*(A52-$J$8)/16</f>
+        <f t="shared" ref="C52:C66" si="8">$K$8 + ($K$9-$K$8)*(A52-$J$8)/16</f>
         <v>7.0621778264910704</v>
       </c>
       <c r="D52">
@@ -6944,7 +7138,7 @@
         <v>7.1414284285428504</v>
       </c>
       <c r="C53" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.1291651245988508</v>
       </c>
       <c r="D53">
@@ -6962,7 +7156,7 @@
         <v>7.2111025509279782</v>
       </c>
       <c r="C54" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.196152422706632</v>
       </c>
       <c r="D54">
@@ -6980,7 +7174,7 @@
         <v>7.2801098892805181</v>
       </c>
       <c r="C55" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.2631397208144124</v>
       </c>
       <c r="D55">
@@ -6998,7 +7192,7 @@
         <v>7.3484692283495345</v>
       </c>
       <c r="C56" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.3301270189221928</v>
       </c>
       <c r="D56">
@@ -7016,7 +7210,7 @@
         <v>7.416198487095663</v>
       </c>
       <c r="C57" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.397114317029974</v>
       </c>
       <c r="D57">
@@ -7034,7 +7228,7 @@
         <v>7.4833147735478827</v>
       </c>
       <c r="C58" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.4641016151377544</v>
       </c>
       <c r="D58">
@@ -7052,7 +7246,7 @@
         <v>7.5498344352707498</v>
       </c>
       <c r="C59" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.5310889132455348</v>
       </c>
       <c r="D59">
@@ -7070,7 +7264,7 @@
         <v>7.6157731058639087</v>
       </c>
       <c r="C60" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.598076211353316</v>
       </c>
       <c r="D60">
@@ -7088,7 +7282,7 @@
         <v>7.6811457478686078</v>
       </c>
       <c r="C61" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.6650635094610964</v>
       </c>
       <c r="D61">
@@ -7106,7 +7300,7 @@
         <v>7.745966692414834</v>
       </c>
       <c r="C62" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.7320508075688767</v>
       </c>
       <c r="D62">
@@ -7124,7 +7318,7 @@
         <v>7.810249675906654</v>
       </c>
       <c r="C63" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.799038105676658</v>
       </c>
       <c r="D63">
@@ -7142,7 +7336,7 @@
         <v>7.8740078740118111</v>
       </c>
       <c r="C64" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.8660254037844384</v>
       </c>
       <c r="D64">
@@ -7160,7 +7354,7 @@
         <v>7.9372539331937721</v>
       </c>
       <c r="C65" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.9330127018922187</v>
       </c>
       <c r="D65">
@@ -7174,11 +7368,11 @@
         <v>64</v>
       </c>
       <c r="B66" s="14">
-        <f t="shared" ref="B66:B128" si="8">SQRT(A66)</f>
+        <f t="shared" ref="B66:B128" si="9">SQRT(A66)</f>
         <v>8</v>
       </c>
       <c r="C66" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="D66">
@@ -7192,7 +7386,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.0622577482985491</v>
       </c>
       <c r="C67" s="5">
@@ -7200,287 +7394,287 @@
         <v>8.0590169943749466</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D129" si="9">ABS(B67-C67)</f>
+        <f t="shared" ref="D67:D129" si="10">ABS(B67-C67)</f>
         <v>3.2407539236025684E-3</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="5">
-        <f t="shared" ref="A68:A129" si="10">A67+1</f>
+        <f t="shared" ref="A68:A129" si="11">A67+1</f>
         <v>66</v>
       </c>
       <c r="B68" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.1240384046359608</v>
       </c>
       <c r="C68" s="5">
-        <f t="shared" ref="C68:C82" si="11">$K$9 + ($K$10-$K$9)*(A68-$J$9)/16</f>
+        <f t="shared" ref="C68:C82" si="12">$K$9 + ($K$10-$K$9)*(A68-$J$9)/16</f>
         <v>8.1180339887498949</v>
       </c>
       <c r="D68">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.004415886065928E-3</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
+        <f t="shared" si="11"/>
+        <v>67</v>
+      </c>
+      <c r="B69" s="5">
+        <f t="shared" si="9"/>
+        <v>8.1853527718724504</v>
+      </c>
+      <c r="C69" s="5">
+        <f t="shared" si="12"/>
+        <v>8.1770509831248432</v>
+      </c>
+      <c r="D69">
         <f t="shared" si="10"/>
-        <v>67</v>
-      </c>
-      <c r="B69" s="5">
-        <f t="shared" si="8"/>
-        <v>8.1853527718724504</v>
-      </c>
-      <c r="C69" s="5">
-        <f t="shared" si="11"/>
-        <v>8.1770509831248432</v>
-      </c>
-      <c r="D69">
-        <f t="shared" si="9"/>
         <v>8.3017887476071195E-3</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="5">
+        <f t="shared" si="11"/>
+        <v>68</v>
+      </c>
+      <c r="B70" s="5">
+        <f t="shared" si="9"/>
+        <v>8.2462112512353212</v>
+      </c>
+      <c r="C70" s="5">
+        <f t="shared" si="12"/>
+        <v>8.2360679774997898</v>
+      </c>
+      <c r="D70">
         <f t="shared" si="10"/>
-        <v>68</v>
-      </c>
-      <c r="B70" s="5">
-        <f t="shared" si="8"/>
-        <v>8.2462112512353212</v>
-      </c>
-      <c r="C70" s="5">
-        <f t="shared" si="11"/>
-        <v>8.2360679774997898</v>
-      </c>
-      <c r="D70">
-        <f t="shared" si="9"/>
         <v>1.0143273735531366E-2</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
+        <f t="shared" si="11"/>
+        <v>69</v>
+      </c>
+      <c r="B71" s="5">
+        <f t="shared" si="9"/>
+        <v>8.3066238629180749</v>
+      </c>
+      <c r="C71" s="5">
+        <f t="shared" si="12"/>
+        <v>8.2950849718747364</v>
+      </c>
+      <c r="D71">
         <f t="shared" si="10"/>
-        <v>69</v>
-      </c>
-      <c r="B71" s="5">
-        <f t="shared" si="8"/>
-        <v>8.3066238629180749</v>
-      </c>
-      <c r="C71" s="5">
-        <f t="shared" si="11"/>
-        <v>8.2950849718747364</v>
-      </c>
-      <c r="D71">
-        <f t="shared" si="9"/>
         <v>1.1538891043338495E-2</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="5">
+        <f t="shared" si="11"/>
+        <v>70</v>
+      </c>
+      <c r="B72" s="5">
+        <f t="shared" si="9"/>
+        <v>8.3666002653407556</v>
+      </c>
+      <c r="C72" s="5">
+        <f t="shared" si="12"/>
+        <v>8.3541019662496847</v>
+      </c>
+      <c r="D72">
         <f t="shared" si="10"/>
-        <v>70</v>
-      </c>
-      <c r="B72" s="5">
-        <f t="shared" si="8"/>
-        <v>8.3666002653407556</v>
-      </c>
-      <c r="C72" s="5">
-        <f t="shared" si="11"/>
-        <v>8.3541019662496847</v>
-      </c>
-      <c r="D72">
-        <f t="shared" si="9"/>
         <v>1.2498299091070919E-2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="5">
+        <f t="shared" si="11"/>
+        <v>71</v>
+      </c>
+      <c r="B73" s="5">
+        <f t="shared" si="9"/>
+        <v>8.426149773176359</v>
+      </c>
+      <c r="C73" s="5">
+        <f t="shared" si="12"/>
+        <v>8.413118960624633</v>
+      </c>
+      <c r="D73">
         <f t="shared" si="10"/>
-        <v>71</v>
-      </c>
-      <c r="B73" s="5">
-        <f t="shared" si="8"/>
-        <v>8.426149773176359</v>
-      </c>
-      <c r="C73" s="5">
-        <f t="shared" si="11"/>
-        <v>8.413118960624633</v>
-      </c>
-      <c r="D73">
-        <f t="shared" si="9"/>
         <v>1.3030812551726001E-2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
+        <f t="shared" si="11"/>
+        <v>72</v>
+      </c>
+      <c r="B74" s="5">
+        <f t="shared" si="9"/>
+        <v>8.4852813742385695</v>
+      </c>
+      <c r="C74" s="5">
+        <f t="shared" si="12"/>
+        <v>8.4721359549995796</v>
+      </c>
+      <c r="D74">
         <f t="shared" si="10"/>
-        <v>72</v>
-      </c>
-      <c r="B74" s="5">
-        <f t="shared" si="8"/>
-        <v>8.4852813742385695</v>
-      </c>
-      <c r="C74" s="5">
-        <f t="shared" si="11"/>
-        <v>8.4721359549995796</v>
-      </c>
-      <c r="D74">
-        <f t="shared" si="9"/>
         <v>1.314541923898993E-2</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="5">
+        <f t="shared" si="11"/>
+        <v>73</v>
+      </c>
+      <c r="B75" s="5">
+        <f t="shared" si="9"/>
+        <v>8.5440037453175304</v>
+      </c>
+      <c r="C75" s="5">
+        <f t="shared" si="12"/>
+        <v>8.5311529493745262</v>
+      </c>
+      <c r="D75">
         <f t="shared" si="10"/>
-        <v>73</v>
-      </c>
-      <c r="B75" s="5">
-        <f t="shared" si="8"/>
-        <v>8.5440037453175304</v>
-      </c>
-      <c r="C75" s="5">
-        <f t="shared" si="11"/>
-        <v>8.5311529493745262</v>
-      </c>
-      <c r="D75">
-        <f t="shared" si="9"/>
         <v>1.2850795943004201E-2</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="5">
+        <f t="shared" si="11"/>
+        <v>74</v>
+      </c>
+      <c r="B76" s="5">
+        <f t="shared" si="9"/>
+        <v>8.6023252670426267</v>
+      </c>
+      <c r="C76" s="5">
+        <f t="shared" si="12"/>
+        <v>8.5901699437494745</v>
+      </c>
+      <c r="D76">
         <f t="shared" si="10"/>
-        <v>74</v>
-      </c>
-      <c r="B76" s="5">
-        <f t="shared" si="8"/>
-        <v>8.6023252670426267</v>
-      </c>
-      <c r="C76" s="5">
-        <f t="shared" si="11"/>
-        <v>8.5901699437494745</v>
-      </c>
-      <c r="D76">
-        <f t="shared" si="9"/>
         <v>1.2155323293152165E-2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="5">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
+      <c r="B77" s="5">
+        <f t="shared" si="9"/>
+        <v>8.6602540378443873</v>
+      </c>
+      <c r="C77" s="5">
+        <f t="shared" si="12"/>
+        <v>8.6491869381244229</v>
+      </c>
+      <c r="D77">
         <f t="shared" si="10"/>
-        <v>75</v>
-      </c>
-      <c r="B77" s="5">
-        <f t="shared" si="8"/>
-        <v>8.6602540378443873</v>
-      </c>
-      <c r="C77" s="5">
-        <f t="shared" si="11"/>
-        <v>8.6491869381244229</v>
-      </c>
-      <c r="D77">
-        <f t="shared" si="9"/>
         <v>1.1067099719964446E-2</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="5">
+        <f t="shared" si="11"/>
+        <v>76</v>
+      </c>
+      <c r="B78" s="5">
+        <f t="shared" si="9"/>
+        <v>8.717797887081348</v>
+      </c>
+      <c r="C78" s="5">
+        <f t="shared" si="12"/>
+        <v>8.7082039324993694</v>
+      </c>
+      <c r="D78">
         <f t="shared" si="10"/>
-        <v>76</v>
-      </c>
-      <c r="B78" s="5">
-        <f t="shared" si="8"/>
-        <v>8.717797887081348</v>
-      </c>
-      <c r="C78" s="5">
-        <f t="shared" si="11"/>
-        <v>8.7082039324993694</v>
-      </c>
-      <c r="D78">
-        <f t="shared" si="9"/>
         <v>9.5939545819785366E-3</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="5">
+        <f t="shared" si="11"/>
+        <v>77</v>
+      </c>
+      <c r="B79" s="5">
+        <f t="shared" si="9"/>
+        <v>8.7749643873921226</v>
+      </c>
+      <c r="C79" s="5">
+        <f t="shared" si="12"/>
+        <v>8.767220926874316</v>
+      </c>
+      <c r="D79">
         <f t="shared" si="10"/>
-        <v>77</v>
-      </c>
-      <c r="B79" s="5">
-        <f t="shared" si="8"/>
-        <v>8.7749643873921226</v>
-      </c>
-      <c r="C79" s="5">
-        <f t="shared" si="11"/>
-        <v>8.767220926874316</v>
-      </c>
-      <c r="D79">
-        <f t="shared" si="9"/>
         <v>7.7434605178066107E-3</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
+        <f t="shared" si="11"/>
+        <v>78</v>
+      </c>
+      <c r="B80" s="5">
+        <f t="shared" si="9"/>
+        <v>8.8317608663278477</v>
+      </c>
+      <c r="C80" s="5">
+        <f t="shared" si="12"/>
+        <v>8.8262379212492643</v>
+      </c>
+      <c r="D80">
         <f t="shared" si="10"/>
-        <v>78</v>
-      </c>
-      <c r="B80" s="5">
-        <f t="shared" si="8"/>
-        <v>8.8317608663278477</v>
-      </c>
-      <c r="C80" s="5">
-        <f t="shared" si="11"/>
-        <v>8.8262379212492643</v>
-      </c>
-      <c r="D80">
-        <f t="shared" si="9"/>
         <v>5.5229450785834189E-3</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
+        <f t="shared" si="11"/>
+        <v>79</v>
+      </c>
+      <c r="B81" s="5">
+        <f t="shared" si="9"/>
+        <v>8.8881944173155887</v>
+      </c>
+      <c r="C81" s="5">
+        <f t="shared" si="12"/>
+        <v>8.8852549156242127</v>
+      </c>
+      <c r="D81">
         <f t="shared" si="10"/>
-        <v>79</v>
-      </c>
-      <c r="B81" s="5">
-        <f t="shared" si="8"/>
-        <v>8.8881944173155887</v>
-      </c>
-      <c r="C81" s="5">
-        <f t="shared" si="11"/>
-        <v>8.8852549156242127</v>
-      </c>
-      <c r="D81">
-        <f t="shared" si="9"/>
         <v>2.939501691376023E-3</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="5">
+        <f t="shared" si="11"/>
+        <v>80</v>
+      </c>
+      <c r="B82" s="5">
+        <f t="shared" si="9"/>
+        <v>8.9442719099991592</v>
+      </c>
+      <c r="C82" s="5">
+        <f t="shared" si="12"/>
+        <v>8.9442719099991592</v>
+      </c>
+      <c r="D82">
         <f t="shared" si="10"/>
-        <v>80</v>
-      </c>
-      <c r="B82" s="5">
-        <f t="shared" si="8"/>
-        <v>8.9442719099991592</v>
-      </c>
-      <c r="C82" s="5">
-        <f t="shared" si="11"/>
-        <v>8.9442719099991592</v>
-      </c>
-      <c r="D82">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>81</v>
       </c>
       <c r="B83" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="C83" s="6">
@@ -7488,287 +7682,287 @@
         <v>8.9976273513200056</v>
       </c>
       <c r="D83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.3726486799944269E-3</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="6">
+        <f t="shared" si="11"/>
+        <v>82</v>
+      </c>
+      <c r="B84" s="6">
+        <f t="shared" si="9"/>
+        <v>9.0553851381374173</v>
+      </c>
+      <c r="C84" s="6">
+        <f t="shared" ref="C84:C98" si="13">$K$10 + ($K$11-$K$10)*(A84-$J$10)/16</f>
+        <v>9.0509827926408537</v>
+      </c>
+      <c r="D84">
         <f t="shared" si="10"/>
-        <v>82</v>
-      </c>
-      <c r="B84" s="6">
-        <f t="shared" si="8"/>
-        <v>9.0553851381374173</v>
-      </c>
-      <c r="C84" s="6">
-        <f t="shared" ref="C84:C98" si="12">$K$10 + ($K$11-$K$10)*(A84-$J$10)/16</f>
-        <v>9.0509827926408537</v>
-      </c>
-      <c r="D84">
-        <f t="shared" si="9"/>
         <v>4.4023454965635977E-3</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="6">
+        <f t="shared" si="11"/>
+        <v>83</v>
+      </c>
+      <c r="B85" s="6">
+        <f t="shared" si="9"/>
+        <v>9.1104335791442992</v>
+      </c>
+      <c r="C85" s="6">
+        <f t="shared" si="13"/>
+        <v>9.1043382339617001</v>
+      </c>
+      <c r="D85">
         <f t="shared" si="10"/>
-        <v>83</v>
-      </c>
-      <c r="B85" s="6">
-        <f t="shared" si="8"/>
-        <v>9.1104335791442992</v>
-      </c>
-      <c r="C85" s="6">
-        <f t="shared" si="12"/>
-        <v>9.1043382339617001</v>
-      </c>
-      <c r="D85">
-        <f t="shared" si="9"/>
         <v>6.0953451825991323E-3</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="6">
+        <f t="shared" si="11"/>
+        <v>84</v>
+      </c>
+      <c r="B86" s="6">
+        <f t="shared" si="9"/>
+        <v>9.1651513899116797</v>
+      </c>
+      <c r="C86" s="6">
+        <f t="shared" si="13"/>
+        <v>9.1576936752825482</v>
+      </c>
+      <c r="D86">
         <f t="shared" si="10"/>
-        <v>84</v>
-      </c>
-      <c r="B86" s="6">
-        <f t="shared" si="8"/>
-        <v>9.1651513899116797</v>
-      </c>
-      <c r="C86" s="6">
-        <f t="shared" si="12"/>
-        <v>9.1576936752825482</v>
-      </c>
-      <c r="D86">
-        <f t="shared" si="9"/>
         <v>7.4577146291314733E-3</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
+        <f t="shared" si="11"/>
+        <v>85</v>
+      </c>
+      <c r="B87" s="6">
+        <f t="shared" si="9"/>
+        <v>9.2195444572928871</v>
+      </c>
+      <c r="C87" s="6">
+        <f t="shared" si="13"/>
+        <v>9.2110491166033945</v>
+      </c>
+      <c r="D87">
         <f t="shared" si="10"/>
-        <v>85</v>
-      </c>
-      <c r="B87" s="6">
-        <f t="shared" si="8"/>
-        <v>9.2195444572928871</v>
-      </c>
-      <c r="C87" s="6">
-        <f t="shared" si="12"/>
-        <v>9.2110491166033945</v>
-      </c>
-      <c r="D87">
-        <f t="shared" si="9"/>
         <v>8.4953406894925365E-3</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
+        <f t="shared" si="11"/>
+        <v>86</v>
+      </c>
+      <c r="B88" s="6">
+        <f t="shared" si="9"/>
+        <v>9.2736184954957039</v>
+      </c>
+      <c r="C88" s="6">
+        <f t="shared" si="13"/>
+        <v>9.2644045579242409</v>
+      </c>
+      <c r="D88">
         <f t="shared" si="10"/>
-        <v>86</v>
-      </c>
-      <c r="B88" s="6">
-        <f t="shared" si="8"/>
-        <v>9.2736184954957039</v>
-      </c>
-      <c r="C88" s="6">
-        <f t="shared" si="12"/>
-        <v>9.2644045579242409</v>
-      </c>
-      <c r="D88">
-        <f t="shared" si="9"/>
         <v>9.2139375714630489E-3</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="6">
+        <f t="shared" si="11"/>
+        <v>87</v>
+      </c>
+      <c r="B89" s="6">
+        <f t="shared" si="9"/>
+        <v>9.3273790530888157</v>
+      </c>
+      <c r="C89" s="6">
+        <f t="shared" si="13"/>
+        <v>9.317759999245089</v>
+      </c>
+      <c r="D89">
         <f t="shared" si="10"/>
-        <v>87</v>
-      </c>
-      <c r="B89" s="6">
-        <f t="shared" si="8"/>
-        <v>9.3273790530888157</v>
-      </c>
-      <c r="C89" s="6">
-        <f t="shared" si="12"/>
-        <v>9.317759999245089</v>
-      </c>
-      <c r="D89">
-        <f t="shared" si="9"/>
         <v>9.6190538437266326E-3</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="6">
+        <f t="shared" si="11"/>
+        <v>88</v>
+      </c>
+      <c r="B90" s="6">
+        <f t="shared" si="9"/>
+        <v>9.3808315196468595</v>
+      </c>
+      <c r="C90" s="6">
+        <f t="shared" si="13"/>
+        <v>9.3711154405659354</v>
+      </c>
+      <c r="D90">
         <f t="shared" si="10"/>
-        <v>88</v>
-      </c>
-      <c r="B90" s="6">
-        <f t="shared" si="8"/>
-        <v>9.3808315196468595</v>
-      </c>
-      <c r="C90" s="6">
-        <f t="shared" si="12"/>
-        <v>9.3711154405659354</v>
-      </c>
-      <c r="D90">
-        <f t="shared" si="9"/>
         <v>9.7160790809240893E-3</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
+        <f t="shared" si="11"/>
+        <v>89</v>
+      </c>
+      <c r="B91" s="6">
+        <f t="shared" si="9"/>
+        <v>9.4339811320566032</v>
+      </c>
+      <c r="C91" s="6">
+        <f t="shared" si="13"/>
+        <v>9.4244708818867817</v>
+      </c>
+      <c r="D91">
         <f t="shared" si="10"/>
-        <v>89</v>
-      </c>
-      <c r="B91" s="6">
-        <f t="shared" si="8"/>
-        <v>9.4339811320566032</v>
-      </c>
-      <c r="C91" s="6">
-        <f t="shared" si="12"/>
-        <v>9.4244708818867817</v>
-      </c>
-      <c r="D91">
-        <f t="shared" si="9"/>
         <v>9.5102501698214326E-3</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
+        <f t="shared" si="11"/>
+        <v>90</v>
+      </c>
+      <c r="B92" s="6">
+        <f t="shared" si="9"/>
+        <v>9.4868329805051381</v>
+      </c>
+      <c r="C92" s="6">
+        <f t="shared" si="13"/>
+        <v>9.4778263232076299</v>
+      </c>
+      <c r="D92">
         <f t="shared" si="10"/>
-        <v>90</v>
-      </c>
-      <c r="B92" s="6">
-        <f t="shared" si="8"/>
-        <v>9.4868329805051381</v>
-      </c>
-      <c r="C92" s="6">
-        <f t="shared" si="12"/>
-        <v>9.4778263232076299</v>
-      </c>
-      <c r="D92">
-        <f t="shared" si="9"/>
         <v>9.0066572975082693E-3</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="6">
+        <f t="shared" si="11"/>
+        <v>91</v>
+      </c>
+      <c r="B93" s="6">
+        <f t="shared" si="9"/>
+        <v>9.5393920141694561</v>
+      </c>
+      <c r="C93" s="6">
+        <f t="shared" si="13"/>
+        <v>9.5311817645284762</v>
+      </c>
+      <c r="D93">
         <f t="shared" si="10"/>
-        <v>91</v>
-      </c>
-      <c r="B93" s="6">
-        <f t="shared" si="8"/>
-        <v>9.5393920141694561</v>
-      </c>
-      <c r="C93" s="6">
-        <f t="shared" si="12"/>
-        <v>9.5311817645284762</v>
-      </c>
-      <c r="D93">
-        <f t="shared" si="9"/>
         <v>8.2102496409799386E-3</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
+        <f t="shared" si="11"/>
+        <v>92</v>
+      </c>
+      <c r="B94" s="6">
+        <f t="shared" si="9"/>
+        <v>9.5916630466254382</v>
+      </c>
+      <c r="C94" s="6">
+        <f t="shared" si="13"/>
+        <v>9.5845372058493226</v>
+      </c>
+      <c r="D94">
         <f t="shared" si="10"/>
-        <v>92</v>
-      </c>
-      <c r="B94" s="6">
-        <f t="shared" si="8"/>
-        <v>9.5916630466254382</v>
-      </c>
-      <c r="C94" s="6">
-        <f t="shared" si="12"/>
-        <v>9.5845372058493226</v>
-      </c>
-      <c r="D94">
-        <f t="shared" si="9"/>
         <v>7.1258407761156661E-3</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
+        <f t="shared" si="11"/>
+        <v>93</v>
+      </c>
+      <c r="B95" s="6">
+        <f t="shared" si="9"/>
+        <v>9.6436507609929549</v>
+      </c>
+      <c r="C95" s="6">
+        <f t="shared" si="13"/>
+        <v>9.6378926471701707</v>
+      </c>
+      <c r="D95">
         <f t="shared" si="10"/>
-        <v>93</v>
-      </c>
-      <c r="B95" s="6">
-        <f t="shared" si="8"/>
-        <v>9.6436507609929549</v>
-      </c>
-      <c r="C95" s="6">
-        <f t="shared" si="12"/>
-        <v>9.6378926471701707</v>
-      </c>
-      <c r="D95">
-        <f t="shared" si="9"/>
         <v>5.7581138227842388E-3</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
+        <f t="shared" si="11"/>
+        <v>94</v>
+      </c>
+      <c r="B96" s="6">
+        <f t="shared" si="9"/>
+        <v>9.6953597148326587</v>
+      </c>
+      <c r="C96" s="6">
+        <f t="shared" si="13"/>
+        <v>9.691248088491017</v>
+      </c>
+      <c r="D96">
         <f t="shared" si="10"/>
-        <v>94</v>
-      </c>
-      <c r="B96" s="6">
-        <f t="shared" si="8"/>
-        <v>9.6953597148326587</v>
-      </c>
-      <c r="C96" s="6">
-        <f t="shared" si="12"/>
-        <v>9.691248088491017</v>
-      </c>
-      <c r="D96">
-        <f t="shared" si="9"/>
         <v>4.1116263416416388E-3</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="6">
+        <f t="shared" si="11"/>
+        <v>95</v>
+      </c>
+      <c r="B97" s="6">
+        <f t="shared" si="9"/>
+        <v>9.7467943448089631</v>
+      </c>
+      <c r="C97" s="6">
+        <f t="shared" si="13"/>
+        <v>9.7446035298118652</v>
+      </c>
+      <c r="D97">
         <f t="shared" si="10"/>
-        <v>95</v>
-      </c>
-      <c r="B97" s="6">
-        <f t="shared" si="8"/>
-        <v>9.7467943448089631</v>
-      </c>
-      <c r="C97" s="6">
-        <f t="shared" si="12"/>
-        <v>9.7446035298118652</v>
-      </c>
-      <c r="D97">
-        <f t="shared" si="9"/>
         <v>2.1908149970979451E-3</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
+        <f t="shared" si="11"/>
+        <v>96</v>
+      </c>
+      <c r="B98" s="6">
+        <f t="shared" si="9"/>
+        <v>9.7979589711327115</v>
+      </c>
+      <c r="C98" s="6">
+        <f t="shared" si="13"/>
+        <v>9.7979589711327115</v>
+      </c>
+      <c r="D98">
         <f t="shared" si="10"/>
-        <v>96</v>
-      </c>
-      <c r="B98" s="6">
-        <f t="shared" si="8"/>
-        <v>9.7979589711327115</v>
-      </c>
-      <c r="C98" s="6">
-        <f t="shared" si="12"/>
-        <v>9.7979589711327115</v>
-      </c>
-      <c r="D98">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>97</v>
       </c>
       <c r="B99" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>9.8488578017961039</v>
       </c>
       <c r="C99" s="7">
@@ -7776,287 +7970,287 @@
         <v>9.8470243632030652</v>
       </c>
       <c r="D99">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.8334385930387498E-3</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
+        <f t="shared" si="11"/>
+        <v>98</v>
+      </c>
+      <c r="B100" s="7">
+        <f t="shared" si="9"/>
+        <v>9.8994949366116654</v>
+      </c>
+      <c r="C100" s="7">
+        <f t="shared" ref="C100:C114" si="14">$K$11 + ($K$12-$K$11)*(A100-$J$11)/16</f>
+        <v>9.8960897552734188</v>
+      </c>
+      <c r="D100">
         <f t="shared" si="10"/>
-        <v>98</v>
-      </c>
-      <c r="B100" s="7">
-        <f t="shared" si="8"/>
-        <v>9.8994949366116654</v>
-      </c>
-      <c r="C100" s="7">
-        <f t="shared" ref="C100:C114" si="13">$K$11 + ($K$12-$K$11)*(A100-$J$11)/16</f>
-        <v>9.8960897552734188</v>
-      </c>
-      <c r="D100">
-        <f t="shared" si="9"/>
         <v>3.4051813382465212E-3</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="7">
+        <f t="shared" si="11"/>
+        <v>99</v>
+      </c>
+      <c r="B101" s="7">
+        <f t="shared" si="9"/>
+        <v>9.9498743710661994</v>
+      </c>
+      <c r="C101" s="7">
+        <f t="shared" si="14"/>
+        <v>9.9451551473437707</v>
+      </c>
+      <c r="D101">
         <f t="shared" si="10"/>
-        <v>99</v>
-      </c>
-      <c r="B101" s="7">
-        <f t="shared" si="8"/>
-        <v>9.9498743710661994</v>
-      </c>
-      <c r="C101" s="7">
-        <f t="shared" si="13"/>
-        <v>9.9451551473437707</v>
-      </c>
-      <c r="D101">
-        <f t="shared" si="9"/>
         <v>4.7192237224287226E-3</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="7">
+        <f t="shared" si="11"/>
+        <v>100</v>
+      </c>
+      <c r="B102" s="7">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="C102" s="7">
+        <f t="shared" si="14"/>
+        <v>9.9942205394141244</v>
+      </c>
+      <c r="D102">
         <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="B102" s="7">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="C102" s="7">
-        <f t="shared" si="13"/>
-        <v>9.9942205394141244</v>
-      </c>
-      <c r="D102">
-        <f t="shared" si="9"/>
         <v>5.7794605858756398E-3</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
+        <f t="shared" si="11"/>
+        <v>101</v>
+      </c>
+      <c r="B103" s="7">
+        <f t="shared" si="9"/>
+        <v>10.04987562112089</v>
+      </c>
+      <c r="C103" s="7">
+        <f t="shared" si="14"/>
+        <v>10.043285931484478</v>
+      </c>
+      <c r="D103">
         <f t="shared" si="10"/>
-        <v>101</v>
-      </c>
-      <c r="B103" s="7">
-        <f t="shared" si="8"/>
-        <v>10.04987562112089</v>
-      </c>
-      <c r="C103" s="7">
-        <f t="shared" si="13"/>
-        <v>10.043285931484478</v>
-      </c>
-      <c r="D103">
-        <f t="shared" si="9"/>
         <v>6.5896896364119328E-3</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="7">
+        <f t="shared" si="11"/>
+        <v>102</v>
+      </c>
+      <c r="B104" s="7">
+        <f t="shared" si="9"/>
+        <v>10.099504938362077</v>
+      </c>
+      <c r="C104" s="7">
+        <f t="shared" si="14"/>
+        <v>10.09235132355483</v>
+      </c>
+      <c r="D104">
         <f t="shared" si="10"/>
-        <v>102</v>
-      </c>
-      <c r="B104" s="7">
-        <f t="shared" si="8"/>
-        <v>10.099504938362077</v>
-      </c>
-      <c r="C104" s="7">
-        <f t="shared" si="13"/>
-        <v>10.09235132355483</v>
-      </c>
-      <c r="D104">
-        <f t="shared" si="9"/>
         <v>7.1536148072475214E-3</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
+        <f t="shared" si="11"/>
+        <v>103</v>
+      </c>
+      <c r="B105" s="7">
+        <f t="shared" si="9"/>
+        <v>10.148891565092219</v>
+      </c>
+      <c r="C105" s="7">
+        <f t="shared" si="14"/>
+        <v>10.141416715625184</v>
+      </c>
+      <c r="D105">
         <f t="shared" si="10"/>
-        <v>103</v>
-      </c>
-      <c r="B105" s="7">
-        <f t="shared" si="8"/>
-        <v>10.148891565092219</v>
-      </c>
-      <c r="C105" s="7">
-        <f t="shared" si="13"/>
-        <v>10.141416715625184</v>
-      </c>
-      <c r="D105">
-        <f t="shared" si="9"/>
         <v>7.4748494670355825E-3</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="7">
+        <f t="shared" si="11"/>
+        <v>104</v>
+      </c>
+      <c r="B106" s="7">
+        <f t="shared" si="9"/>
+        <v>10.198039027185569</v>
+      </c>
+      <c r="C106" s="7">
+        <f t="shared" si="14"/>
+        <v>10.190482107695537</v>
+      </c>
+      <c r="D106">
         <f t="shared" si="10"/>
-        <v>104</v>
-      </c>
-      <c r="B106" s="7">
-        <f t="shared" si="8"/>
-        <v>10.198039027185569</v>
-      </c>
-      <c r="C106" s="7">
-        <f t="shared" si="13"/>
-        <v>10.190482107695537</v>
-      </c>
-      <c r="D106">
-        <f t="shared" si="9"/>
         <v>7.5569194900317882E-3</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
+        <f t="shared" si="11"/>
+        <v>105</v>
+      </c>
+      <c r="B107" s="7">
+        <f t="shared" si="9"/>
+        <v>10.246950765959598</v>
+      </c>
+      <c r="C107" s="7">
+        <f t="shared" si="14"/>
+        <v>10.239547499765891</v>
+      </c>
+      <c r="D107">
         <f t="shared" si="10"/>
-        <v>105</v>
-      </c>
-      <c r="B107" s="7">
-        <f t="shared" si="8"/>
-        <v>10.246950765959598</v>
-      </c>
-      <c r="C107" s="7">
-        <f t="shared" si="13"/>
-        <v>10.239547499765891</v>
-      </c>
-      <c r="D107">
-        <f t="shared" si="9"/>
         <v>7.4032661937071254E-3</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="7">
+        <f t="shared" si="11"/>
+        <v>106</v>
+      </c>
+      <c r="B108" s="7">
+        <f t="shared" si="9"/>
+        <v>10.295630140987001</v>
+      </c>
+      <c r="C108" s="7">
+        <f t="shared" si="14"/>
+        <v>10.288612891836245</v>
+      </c>
+      <c r="D108">
         <f t="shared" si="10"/>
-        <v>106</v>
-      </c>
-      <c r="B108" s="7">
-        <f t="shared" si="8"/>
-        <v>10.295630140987001</v>
-      </c>
-      <c r="C108" s="7">
-        <f t="shared" si="13"/>
-        <v>10.288612891836245</v>
-      </c>
-      <c r="D108">
-        <f t="shared" si="9"/>
         <v>7.0172491507562995E-3</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
+        <f t="shared" si="11"/>
+        <v>107</v>
+      </c>
+      <c r="B109" s="7">
+        <f t="shared" si="9"/>
+        <v>10.344080432788601</v>
+      </c>
+      <c r="C109" s="7">
+        <f t="shared" si="14"/>
+        <v>10.337678283906596</v>
+      </c>
+      <c r="D109">
         <f t="shared" si="10"/>
-        <v>107</v>
-      </c>
-      <c r="B109" s="7">
-        <f t="shared" si="8"/>
-        <v>10.344080432788601</v>
-      </c>
-      <c r="C109" s="7">
-        <f t="shared" si="13"/>
-        <v>10.337678283906596</v>
-      </c>
-      <c r="D109">
-        <f t="shared" si="9"/>
         <v>6.4021488820049655E-3</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
+        <f t="shared" si="11"/>
+        <v>108</v>
+      </c>
+      <c r="B110" s="7">
+        <f t="shared" si="9"/>
+        <v>10.392304845413264</v>
+      </c>
+      <c r="C110" s="7">
+        <f t="shared" si="14"/>
+        <v>10.38674367597695</v>
+      </c>
+      <c r="D110">
         <f t="shared" si="10"/>
-        <v>108</v>
-      </c>
-      <c r="B110" s="7">
-        <f t="shared" si="8"/>
-        <v>10.392304845413264</v>
-      </c>
-      <c r="C110" s="7">
-        <f t="shared" si="13"/>
-        <v>10.38674367597695</v>
-      </c>
-      <c r="D110">
-        <f t="shared" si="9"/>
         <v>5.5611694363140174E-3</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="7">
+        <f t="shared" si="11"/>
+        <v>109</v>
+      </c>
+      <c r="B111" s="7">
+        <f t="shared" si="9"/>
+        <v>10.440306508910551</v>
+      </c>
+      <c r="C111" s="7">
+        <f t="shared" si="14"/>
+        <v>10.435809068047304</v>
+      </c>
+      <c r="D111">
         <f t="shared" si="10"/>
-        <v>109</v>
-      </c>
-      <c r="B111" s="7">
-        <f t="shared" si="8"/>
-        <v>10.440306508910551</v>
-      </c>
-      <c r="C111" s="7">
-        <f t="shared" si="13"/>
-        <v>10.435809068047304</v>
-      </c>
-      <c r="D111">
-        <f t="shared" si="9"/>
         <v>4.4974408632469931E-3</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
+        <f t="shared" si="11"/>
+        <v>110</v>
+      </c>
+      <c r="B112" s="7">
+        <f t="shared" si="9"/>
+        <v>10.488088481701515</v>
+      </c>
+      <c r="C112" s="7">
+        <f t="shared" si="14"/>
+        <v>10.484874460117656</v>
+      </c>
+      <c r="D112">
         <f t="shared" si="10"/>
-        <v>110</v>
-      </c>
-      <c r="B112" s="7">
-        <f t="shared" si="8"/>
-        <v>10.488088481701515</v>
-      </c>
-      <c r="C112" s="7">
-        <f t="shared" si="13"/>
-        <v>10.484874460117656</v>
-      </c>
-      <c r="D112">
-        <f t="shared" si="9"/>
         <v>3.2140215838598607E-3</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
+        <f t="shared" si="11"/>
+        <v>111</v>
+      </c>
+      <c r="B113" s="7">
+        <f t="shared" si="9"/>
+        <v>10.535653752852738</v>
+      </c>
+      <c r="C113" s="7">
+        <f t="shared" si="14"/>
+        <v>10.533939852188009</v>
+      </c>
+      <c r="D113">
         <f t="shared" si="10"/>
-        <v>111</v>
-      </c>
-      <c r="B113" s="7">
-        <f t="shared" si="8"/>
-        <v>10.535653752852738</v>
-      </c>
-      <c r="C113" s="7">
-        <f t="shared" si="13"/>
-        <v>10.533939852188009</v>
-      </c>
-      <c r="D113">
-        <f t="shared" si="9"/>
         <v>1.7139006647290955E-3</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="7">
+        <f t="shared" si="11"/>
+        <v>112</v>
+      </c>
+      <c r="B114" s="7">
+        <f t="shared" si="9"/>
+        <v>10.583005244258363</v>
+      </c>
+      <c r="C114" s="7">
+        <f t="shared" si="14"/>
+        <v>10.583005244258363</v>
+      </c>
+      <c r="D114">
         <f t="shared" si="10"/>
-        <v>112</v>
-      </c>
-      <c r="B114" s="7">
-        <f t="shared" si="8"/>
-        <v>10.583005244258363</v>
-      </c>
-      <c r="C114" s="7">
-        <f t="shared" si="13"/>
-        <v>10.583005244258363</v>
-      </c>
-      <c r="D114">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>113</v>
       </c>
       <c r="B115" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10.63014581273465</v>
       </c>
       <c r="C115" s="13">
@@ -8064,247 +8258,247 @@
         <v>10.628674197678762</v>
       </c>
       <c r="D115">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.471615055887554E-3</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="13">
+        <f t="shared" si="11"/>
+        <v>114</v>
+      </c>
+      <c r="B116" s="13">
+        <f t="shared" si="9"/>
+        <v>10.677078252031311</v>
+      </c>
+      <c r="C116" s="13">
+        <f t="shared" ref="C116:C129" si="15">$K$12 + ($K$13-$K$12)*(A116-$J$12)/16</f>
+        <v>10.674343151099162</v>
+      </c>
+      <c r="D116">
         <f t="shared" si="10"/>
-        <v>114</v>
-      </c>
-      <c r="B116" s="13">
-        <f t="shared" si="8"/>
-        <v>10.677078252031311</v>
-      </c>
-      <c r="C116" s="13">
-        <f t="shared" ref="C116:C129" si="14">$K$12 + ($K$13-$K$12)*(A116-$J$12)/16</f>
-        <v>10.674343151099162</v>
-      </c>
-      <c r="D116">
-        <f t="shared" si="9"/>
         <v>2.735100932149237E-3</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="13">
+        <f t="shared" si="11"/>
+        <v>115</v>
+      </c>
+      <c r="B117" s="13">
+        <f t="shared" si="9"/>
+        <v>10.723805294763608</v>
+      </c>
+      <c r="C117" s="13">
+        <f t="shared" si="15"/>
+        <v>10.720012104519563</v>
+      </c>
+      <c r="D117">
         <f t="shared" si="10"/>
-        <v>115</v>
-      </c>
-      <c r="B117" s="13">
-        <f t="shared" si="8"/>
-        <v>10.723805294763608</v>
-      </c>
-      <c r="C117" s="13">
-        <f t="shared" si="14"/>
-        <v>10.720012104519563</v>
-      </c>
-      <c r="D117">
-        <f t="shared" si="9"/>
         <v>3.7931902440444532E-3</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="13">
+        <f t="shared" si="11"/>
+        <v>116</v>
+      </c>
+      <c r="B118" s="13">
+        <f t="shared" si="9"/>
+        <v>10.770329614269007</v>
+      </c>
+      <c r="C118" s="13">
+        <f t="shared" si="15"/>
+        <v>10.765681057939963</v>
+      </c>
+      <c r="D118">
         <f t="shared" si="10"/>
-        <v>116</v>
-      </c>
-      <c r="B118" s="13">
-        <f t="shared" si="8"/>
-        <v>10.770329614269007</v>
-      </c>
-      <c r="C118" s="13">
-        <f t="shared" si="14"/>
-        <v>10.765681057939963</v>
-      </c>
-      <c r="D118">
-        <f t="shared" si="9"/>
         <v>4.6485563290445953E-3</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="13">
+        <f t="shared" si="11"/>
+        <v>117</v>
+      </c>
+      <c r="B119" s="13">
+        <f t="shared" si="9"/>
+        <v>10.816653826391969</v>
+      </c>
+      <c r="C119" s="13">
+        <f t="shared" si="15"/>
+        <v>10.811350011360362</v>
+      </c>
+      <c r="D119">
         <f t="shared" si="10"/>
-        <v>117</v>
-      </c>
-      <c r="B119" s="13">
-        <f t="shared" si="8"/>
-        <v>10.816653826391969</v>
-      </c>
-      <c r="C119" s="13">
-        <f t="shared" si="14"/>
-        <v>10.811350011360362</v>
-      </c>
-      <c r="D119">
-        <f t="shared" si="9"/>
         <v>5.3038150316062627E-3</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="13">
+        <f t="shared" si="11"/>
+        <v>118</v>
+      </c>
+      <c r="B120" s="13">
+        <f t="shared" si="9"/>
+        <v>10.862780491200215</v>
+      </c>
+      <c r="C120" s="13">
+        <f t="shared" si="15"/>
+        <v>10.857018964780762</v>
+      </c>
+      <c r="D120">
         <f t="shared" si="10"/>
-        <v>118</v>
-      </c>
-      <c r="B120" s="13">
-        <f t="shared" si="8"/>
-        <v>10.862780491200215</v>
-      </c>
-      <c r="C120" s="13">
-        <f t="shared" si="14"/>
-        <v>10.857018964780762</v>
-      </c>
-      <c r="D120">
-        <f t="shared" si="9"/>
         <v>5.7615264194534888E-3</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="13">
+        <f t="shared" si="11"/>
+        <v>119</v>
+      </c>
+      <c r="B121" s="13">
+        <f t="shared" si="9"/>
+        <v>10.908712114635714</v>
+      </c>
+      <c r="C121" s="13">
+        <f t="shared" si="15"/>
+        <v>10.902687918201162</v>
+      </c>
+      <c r="D121">
         <f t="shared" si="10"/>
-        <v>119</v>
-      </c>
-      <c r="B121" s="13">
-        <f t="shared" si="8"/>
-        <v>10.908712114635714</v>
-      </c>
-      <c r="C121" s="13">
-        <f t="shared" si="14"/>
-        <v>10.902687918201162</v>
-      </c>
-      <c r="D121">
-        <f t="shared" si="9"/>
         <v>6.0241964345522092E-3</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="13">
+        <f t="shared" si="11"/>
+        <v>120</v>
+      </c>
+      <c r="B122" s="13">
+        <f t="shared" si="9"/>
+        <v>10.954451150103322</v>
+      </c>
+      <c r="C122" s="13">
+        <f t="shared" si="15"/>
+        <v>10.948356871621563</v>
+      </c>
+      <c r="D122">
         <f t="shared" si="10"/>
-        <v>120</v>
-      </c>
-      <c r="B122" s="13">
-        <f t="shared" si="8"/>
-        <v>10.954451150103322</v>
-      </c>
-      <c r="C122" s="13">
-        <f t="shared" si="14"/>
-        <v>10.948356871621563</v>
-      </c>
-      <c r="D122">
-        <f t="shared" si="9"/>
         <v>6.0942784817594742E-3</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="13">
+        <f t="shared" si="11"/>
+        <v>121</v>
+      </c>
+      <c r="B123" s="13">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="C123" s="13">
+        <f t="shared" si="15"/>
+        <v>10.994025825041962</v>
+      </c>
+      <c r="D123">
         <f t="shared" si="10"/>
-        <v>121</v>
-      </c>
-      <c r="B123" s="13">
-        <f t="shared" si="8"/>
-        <v>11</v>
-      </c>
-      <c r="C123" s="13">
-        <f t="shared" si="14"/>
-        <v>10.994025825041962</v>
-      </c>
-      <c r="D123">
-        <f t="shared" si="9"/>
         <v>5.974174958037537E-3</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="13">
+        <f t="shared" si="11"/>
+        <v>122</v>
+      </c>
+      <c r="B124" s="13">
+        <f t="shared" si="9"/>
+        <v>11.045361017187261</v>
+      </c>
+      <c r="C124" s="13">
+        <f t="shared" si="15"/>
+        <v>11.039694778462362</v>
+      </c>
+      <c r="D124">
         <f t="shared" si="10"/>
-        <v>122</v>
-      </c>
-      <c r="B124" s="13">
-        <f t="shared" si="8"/>
-        <v>11.045361017187261</v>
-      </c>
-      <c r="C124" s="13">
-        <f t="shared" si="14"/>
-        <v>11.039694778462362</v>
-      </c>
-      <c r="D124">
-        <f t="shared" si="9"/>
         <v>5.6662387248991308E-3</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="13">
+        <f t="shared" si="11"/>
+        <v>123</v>
+      </c>
+      <c r="B125" s="13">
+        <f t="shared" si="9"/>
+        <v>11.090536506409418</v>
+      </c>
+      <c r="C125" s="13">
+        <f t="shared" si="15"/>
+        <v>11.085363731882762</v>
+      </c>
+      <c r="D125">
         <f t="shared" si="10"/>
-        <v>123</v>
-      </c>
-      <c r="B125" s="13">
-        <f t="shared" si="8"/>
-        <v>11.090536506409418</v>
-      </c>
-      <c r="C125" s="13">
-        <f t="shared" si="14"/>
-        <v>11.085363731882762</v>
-      </c>
-      <c r="D125">
-        <f t="shared" si="9"/>
         <v>5.1727745266560987E-3</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="13">
+        <f t="shared" si="11"/>
+        <v>124</v>
+      </c>
+      <c r="B126" s="13">
+        <f t="shared" si="9"/>
+        <v>11.135528725660043</v>
+      </c>
+      <c r="C126" s="13">
+        <f t="shared" si="15"/>
+        <v>11.131032685303161</v>
+      </c>
+      <c r="D126">
         <f t="shared" si="10"/>
-        <v>124</v>
-      </c>
-      <c r="B126" s="13">
-        <f t="shared" si="8"/>
-        <v>11.135528725660043</v>
-      </c>
-      <c r="C126" s="13">
-        <f t="shared" si="14"/>
-        <v>11.131032685303161</v>
-      </c>
-      <c r="D126">
-        <f t="shared" si="9"/>
         <v>4.4960403568818919E-3</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="13">
+        <f t="shared" si="11"/>
+        <v>125</v>
+      </c>
+      <c r="B127" s="13">
+        <f t="shared" si="9"/>
+        <v>11.180339887498949</v>
+      </c>
+      <c r="C127" s="13">
+        <f t="shared" si="15"/>
+        <v>11.176701638723561</v>
+      </c>
+      <c r="D127">
         <f t="shared" si="10"/>
-        <v>125</v>
-      </c>
-      <c r="B127" s="13">
-        <f t="shared" si="8"/>
-        <v>11.180339887498949</v>
-      </c>
-      <c r="C127" s="13">
-        <f t="shared" si="14"/>
-        <v>11.176701638723561</v>
-      </c>
-      <c r="D127">
-        <f t="shared" si="9"/>
         <v>3.6382487753883197E-3</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="13">
+        <f t="shared" si="11"/>
+        <v>126</v>
+      </c>
+      <c r="B128" s="13">
+        <f t="shared" si="9"/>
+        <v>11.224972160321824</v>
+      </c>
+      <c r="C128" s="13">
+        <f t="shared" si="15"/>
+        <v>11.222370592143962</v>
+      </c>
+      <c r="D128">
         <f t="shared" si="10"/>
-        <v>126</v>
-      </c>
-      <c r="B128" s="13">
-        <f t="shared" si="8"/>
-        <v>11.224972160321824</v>
-      </c>
-      <c r="C128" s="13">
-        <f t="shared" si="14"/>
-        <v>11.222370592143962</v>
-      </c>
-      <c r="D128">
-        <f t="shared" si="9"/>
         <v>2.60156817786239E-3</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>127</v>
       </c>
       <c r="B129" s="13">
@@ -8312,11 +8506,11 @@
         <v>11.269427669584644</v>
       </c>
       <c r="C129" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>11.268039545564362</v>
       </c>
       <c r="D129">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.388124020282433E-3</v>
       </c>
     </row>
@@ -8326,4 +8520,590 @@
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+    <col min="9" max="10" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.5703125" customWidth="1"/>
+    <col min="18" max="18" width="25.28515625" customWidth="1"/>
+    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+    </row>
+    <row r="2" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18">
+        <v>127</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>1</v>
+      </c>
+      <c r="B3" s="22">
+        <v>175</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="21">
+        <v>0</v>
+      </c>
+      <c r="E3" s="22" t="str">
+        <f>DEC2BIN(27*D3,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="F3" s="22">
+        <f>BIN2DEC(E3)/2^4</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="22">
+        <f>TRUNC(BIN2DEC(E3)/2^4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="22">
+        <f>B2</f>
+        <v>127</v>
+      </c>
+      <c r="I3" s="22">
+        <f>INDEX($A$2:$B$17,G3+2,2)</f>
+        <v>175</v>
+      </c>
+      <c r="J3" s="22">
+        <f>INDEX($A$2:$B$17,G3+1,2)</f>
+        <v>127</v>
+      </c>
+      <c r="K3" s="22">
+        <f>I3-J3</f>
+        <v>48</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="22">
+        <f>F3-G3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="22" t="str">
+        <f>DEC2BIN(M3*2^4,4)</f>
+        <v>0000</v>
+      </c>
+      <c r="O3" s="22">
+        <f>M3*K3</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="22">
+        <f>H3+O3</f>
+        <v>127</v>
+      </c>
+      <c r="R3" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="22">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25">
+        <v>216</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="26">
+        <v>1</v>
+      </c>
+      <c r="E4" s="25" t="str">
+        <f>DEC2BIN(27*D4,8)</f>
+        <v>00011011</v>
+      </c>
+      <c r="F4" s="25">
+        <f>BIN2DEC(E4)/2^4</f>
+        <v>1.6875</v>
+      </c>
+      <c r="G4" s="25">
+        <f>TRUNC(BIN2DEC(E4)/2^4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="25">
+        <f>B3</f>
+        <v>175</v>
+      </c>
+      <c r="I4" s="25">
+        <f>INDEX($A$2:$B$17,G4+2,2)</f>
+        <v>216</v>
+      </c>
+      <c r="J4" s="25">
+        <f>INDEX($A$2:$B$17,G4+1,2)</f>
+        <v>175</v>
+      </c>
+      <c r="K4" s="25">
+        <f>I4-J4</f>
+        <v>41</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="25">
+        <f>F4-G4</f>
+        <v>0.6875</v>
+      </c>
+      <c r="N4" s="25" t="str">
+        <f>DEC2BIN(M4*2^4,4)</f>
+        <v>1011</v>
+      </c>
+      <c r="O4" s="25">
+        <f>M4*K4</f>
+        <v>28.1875</v>
+      </c>
+      <c r="P4" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="25">
+        <f>H4+O4</f>
+        <v>203.1875</v>
+      </c>
+      <c r="R4" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>3</v>
+      </c>
+      <c r="B5" s="22">
+        <v>244</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="21">
+        <v>2</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25">
+        <v>253</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="26">
+        <v>3</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>5</v>
+      </c>
+      <c r="B7" s="22">
+        <v>244</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="21">
+        <v>4</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>6</v>
+      </c>
+      <c r="B8" s="25">
+        <v>216</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="24">
+        <v>5</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>7</v>
+      </c>
+      <c r="B9" s="22">
+        <v>175</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="21">
+        <v>6</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>8</v>
+      </c>
+      <c r="B10" s="25">
+        <v>127</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="24">
+        <v>7</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>9</v>
+      </c>
+      <c r="B11" s="22">
+        <v>78</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="21">
+        <v>8</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>10</v>
+      </c>
+      <c r="B12" s="25">
+        <v>37</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="24">
+        <v>9</v>
+      </c>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <v>11</v>
+      </c>
+      <c r="B13" s="22">
+        <v>9</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="21">
+        <v>10</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
+        <v>12</v>
+      </c>
+      <c r="B14" s="25">
+        <v>0</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="24">
+        <v>11</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>13</v>
+      </c>
+      <c r="B15" s="22">
+        <v>9</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="21">
+        <v>12</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
+        <v>14</v>
+      </c>
+      <c r="B16" s="25">
+        <v>36</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="24">
+        <v>13</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>15</v>
+      </c>
+      <c r="B17" s="22">
+        <v>78</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="21">
+        <v>14</v>
+      </c>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>